<commit_message>
[GEN MCU] Control MCU pin-map 추가
</commit_message>
<xml_diff>
--- a/1_LF_Generator_MCU/Plasma_LF_MCU_PinMap_20180117.xlsx
+++ b/1_LF_Generator_MCU/Plasma_LF_MCU_PinMap_20180117.xlsx
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pin-map'!$B$15:$AB$79</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="525">
   <si>
     <t>Function</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1769,10 +1769,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Main PCB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1922,6 +1918,182 @@
   </si>
   <si>
     <t>PWR_LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main MCU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control MCU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD0_MFC0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD2_MFC2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD4_PIRANI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jumper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD1_MFC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD3_MFC3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN0_START</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN1_STOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPIB_CS0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPIB_CS1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPIB_CS2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT0_GV0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT1_GV1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT2_GV2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT3_GV3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT4_PUMPV1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT5_PUMPV2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT6_PURGEV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT7_VENTV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT8_LED_START</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT9_LED_STOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPIB_CS3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCIB_TX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCIB_RX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPIB_SIMO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPIB_CLK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2312,7 +2484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2720,9 +2892,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2807,18 +2976,57 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2840,44 +3048,17 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3186,8 +3367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB95"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD23" sqref="AD23"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3247,10 +3428,10 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="173" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="193"/>
+      <c r="C3" s="174"/>
       <c r="D3" s="2">
         <v>128</v>
       </c>
@@ -3278,10 +3459,10 @@
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B4" s="194" t="s">
+      <c r="B4" s="175" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="195"/>
+      <c r="C4" s="176"/>
       <c r="D4" s="3">
         <v>16</v>
       </c>
@@ -3311,10 +3492,10 @@
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B5" s="194" t="s">
+      <c r="B5" s="175" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="195"/>
+      <c r="C5" s="176"/>
       <c r="D5" s="3">
         <v>48</v>
       </c>
@@ -3346,10 +3527,10 @@
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B6" s="194" t="s">
+      <c r="B6" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="195"/>
+      <c r="C6" s="176"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
@@ -3373,10 +3554,10 @@
       <c r="X6" s="18"/>
     </row>
     <row r="7" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="196" t="s">
+      <c r="B7" s="177" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="197"/>
+      <c r="C7" s="178"/>
       <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
@@ -3495,51 +3676,51 @@
     </row>
     <row r="13" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="189" t="s">
+      <c r="B14" s="183" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="185"/>
-      <c r="D14" s="185" t="s">
+      <c r="C14" s="179"/>
+      <c r="D14" s="179" t="s">
         <v>163</v>
       </c>
-      <c r="E14" s="185" t="s">
+      <c r="E14" s="179" t="s">
         <v>165</v>
       </c>
-      <c r="F14" s="186"/>
-      <c r="G14" s="176" t="s">
+      <c r="F14" s="180"/>
+      <c r="G14" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="190"/>
-      <c r="I14" s="176" t="s">
+      <c r="H14" s="185"/>
+      <c r="I14" s="184" t="s">
         <v>311</v>
       </c>
-      <c r="J14" s="190"/>
-      <c r="K14" s="176" t="s">
+      <c r="J14" s="185"/>
+      <c r="K14" s="184" t="s">
         <v>312</v>
       </c>
-      <c r="L14" s="177"/>
+      <c r="L14" s="186"/>
       <c r="M14" s="23"/>
       <c r="N14" s="37"/>
-      <c r="O14" s="176" t="s">
+      <c r="O14" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="177"/>
-      <c r="Q14" s="177" t="s">
+      <c r="P14" s="186"/>
+      <c r="Q14" s="186" t="s">
         <v>162</v>
       </c>
-      <c r="R14" s="177"/>
+      <c r="R14" s="186"/>
       <c r="S14" s="56"/>
       <c r="T14" s="35"/>
-      <c r="V14" s="176" t="s">
+      <c r="V14" s="184" t="s">
         <v>14</v>
       </c>
-      <c r="W14" s="177"/>
-      <c r="X14" s="178" t="s">
+      <c r="W14" s="186"/>
+      <c r="X14" s="190" t="s">
         <v>383</v>
       </c>
-      <c r="Y14" s="179"/>
-      <c r="Z14" s="179"/>
-      <c r="AA14" s="180"/>
+      <c r="Y14" s="191"/>
+      <c r="Z14" s="191"/>
+      <c r="AA14" s="192"/>
     </row>
     <row r="15" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7" t="s">
@@ -3548,7 +3729,7 @@
       <c r="C15" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="191"/>
+      <c r="D15" s="187"/>
       <c r="E15" s="15" t="s">
         <v>248</v>
       </c>
@@ -3626,10 +3807,10 @@
       <c r="D16" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="187" t="s">
+      <c r="E16" s="181" t="s">
         <v>176</v>
       </c>
-      <c r="F16" s="188"/>
+      <c r="F16" s="182"/>
       <c r="G16" s="50"/>
       <c r="H16" s="69"/>
       <c r="I16" s="79"/>
@@ -3721,19 +3902,19 @@
       <c r="AA17" s="39"/>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B18" s="172">
+      <c r="B18" s="171">
         <v>3</v>
       </c>
-      <c r="C18" s="173">
+      <c r="C18" s="172">
         <v>3</v>
       </c>
-      <c r="D18" s="173" t="s">
+      <c r="D18" s="172" t="s">
         <v>150</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="F18" s="168" t="s">
+      <c r="F18" s="167" t="s">
         <v>166</v>
       </c>
       <c r="G18" s="64"/>
@@ -3762,37 +3943,37 @@
         <v>72</v>
       </c>
       <c r="T18" s="18"/>
-      <c r="V18" s="162" t="s">
+      <c r="V18" s="161" t="s">
         <v>166</v>
       </c>
-      <c r="W18" s="158" t="s">
+      <c r="W18" s="157" t="s">
         <v>379</v>
       </c>
-      <c r="X18" s="158" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y18" s="158" t="s">
-        <v>467</v>
-      </c>
-      <c r="Z18" s="158" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA18" s="159"/>
+      <c r="X18" s="157" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y18" s="157" t="s">
+        <v>466</v>
+      </c>
+      <c r="Z18" s="157" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA18" s="158"/>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B19" s="172">
+      <c r="B19" s="171">
         <v>4</v>
       </c>
-      <c r="C19" s="173">
+      <c r="C19" s="172">
         <v>4</v>
       </c>
-      <c r="D19" s="173" t="s">
+      <c r="D19" s="172" t="s">
         <v>151</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="F19" s="168" t="s">
+      <c r="F19" s="167" t="s">
         <v>167</v>
       </c>
       <c r="G19" s="64"/>
@@ -3821,37 +4002,37 @@
         <v>72</v>
       </c>
       <c r="T19" s="18"/>
-      <c r="V19" s="162" t="s">
+      <c r="V19" s="161" t="s">
         <v>167</v>
       </c>
-      <c r="W19" s="158" t="s">
+      <c r="W19" s="157" t="s">
         <v>379</v>
       </c>
-      <c r="X19" s="158" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y19" s="158" t="s">
-        <v>467</v>
-      </c>
-      <c r="Z19" s="158" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA19" s="159"/>
+      <c r="X19" s="157" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y19" s="157" t="s">
+        <v>466</v>
+      </c>
+      <c r="Z19" s="157" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA19" s="158"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B20" s="172">
+      <c r="B20" s="171">
         <v>5</v>
       </c>
-      <c r="C20" s="173">
+      <c r="C20" s="172">
         <v>5</v>
       </c>
-      <c r="D20" s="173" t="s">
+      <c r="D20" s="172" t="s">
         <v>168</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="F20" s="168" t="s">
+      <c r="F20" s="167" t="s">
         <v>171</v>
       </c>
       <c r="G20" s="64"/>
@@ -3878,37 +4059,37 @@
         <v>72</v>
       </c>
       <c r="T20" s="18"/>
-      <c r="V20" s="162" t="s">
+      <c r="V20" s="161" t="s">
         <v>171</v>
       </c>
-      <c r="W20" s="158" t="s">
+      <c r="W20" s="157" t="s">
         <v>379</v>
       </c>
-      <c r="X20" s="158" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y20" s="158" t="s">
-        <v>468</v>
-      </c>
-      <c r="Z20" s="158" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA20" s="159"/>
+      <c r="X20" s="157" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y20" s="157" t="s">
+        <v>467</v>
+      </c>
+      <c r="Z20" s="157" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA20" s="158"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B21" s="172">
+      <c r="B21" s="171">
         <v>6</v>
       </c>
-      <c r="C21" s="173">
+      <c r="C21" s="172">
         <v>6</v>
       </c>
-      <c r="D21" s="173" t="s">
+      <c r="D21" s="172" t="s">
         <v>169</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="F21" s="168" t="s">
+      <c r="F21" s="167" t="s">
         <v>175</v>
       </c>
       <c r="G21" s="64"/>
@@ -3935,22 +4116,22 @@
         <v>72</v>
       </c>
       <c r="T21" s="18"/>
-      <c r="V21" s="162" t="s">
+      <c r="V21" s="161" t="s">
         <v>175</v>
       </c>
-      <c r="W21" s="158" t="s">
+      <c r="W21" s="157" t="s">
         <v>379</v>
       </c>
-      <c r="X21" s="158" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y21" s="158" t="s">
-        <v>468</v>
-      </c>
-      <c r="Z21" s="158" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA21" s="159"/>
+      <c r="X21" s="157" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y21" s="157" t="s">
+        <v>467</v>
+      </c>
+      <c r="Z21" s="157" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA21" s="158"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B22" s="102">
@@ -3962,13 +4143,13 @@
       <c r="D22" s="98" t="s">
         <v>170</v>
       </c>
-      <c r="E22" s="174" t="s">
+      <c r="E22" s="188" t="s">
         <v>177</v>
       </c>
-      <c r="F22" s="175"/>
+      <c r="F22" s="189"/>
       <c r="G22" s="75"/>
       <c r="H22" s="103"/>
-      <c r="I22" s="170"/>
+      <c r="I22" s="169"/>
       <c r="J22" s="103"/>
       <c r="K22" s="75"/>
       <c r="L22" s="104"/>
@@ -3990,7 +4171,7 @@
         <v>257</v>
       </c>
       <c r="T22" s="103"/>
-      <c r="U22" s="171"/>
+      <c r="U22" s="170"/>
       <c r="V22" s="100" t="s">
         <v>170</v>
       </c>
@@ -4080,7 +4261,7 @@
       <c r="AA23" s="39"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B24" s="166">
+      <c r="B24" s="165">
         <v>9</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -4140,7 +4321,7 @@
         <v>22</v>
       </c>
       <c r="X24" s="82" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Y24" s="141" t="s">
         <v>72</v>
@@ -4151,7 +4332,7 @@
       <c r="AA24" s="81"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B25" s="166">
+      <c r="B25" s="165">
         <v>10</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4211,10 +4392,10 @@
         <v>22</v>
       </c>
       <c r="X25" s="82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="Y25" s="141" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="Z25" s="141" t="s">
         <v>72</v>
@@ -4222,7 +4403,7 @@
       <c r="AA25" s="81"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B26" s="166">
+      <c r="B26" s="165">
         <v>11</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -4270,10 +4451,10 @@
         <v>22</v>
       </c>
       <c r="X26" s="82" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="Y26" s="82" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Z26" s="141" t="s">
         <v>72</v>
@@ -4290,10 +4471,10 @@
       <c r="D27" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="E27" s="181" t="s">
+      <c r="E27" s="193" t="s">
         <v>189</v>
       </c>
-      <c r="F27" s="182"/>
+      <c r="F27" s="194"/>
       <c r="G27" s="65"/>
       <c r="H27" s="41"/>
       <c r="I27" s="28"/>
@@ -4309,10 +4490,10 @@
       <c r="S27" s="53"/>
       <c r="T27" s="41"/>
       <c r="V27" s="29"/>
-      <c r="W27" s="155"/>
-      <c r="X27" s="155"/>
-      <c r="Y27" s="155"/>
-      <c r="Z27" s="155"/>
+      <c r="W27" s="154"/>
+      <c r="X27" s="154"/>
+      <c r="Y27" s="154"/>
+      <c r="Z27" s="154"/>
       <c r="AA27" s="41"/>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.3">
@@ -4325,10 +4506,10 @@
       <c r="D28" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="E28" s="181" t="s">
+      <c r="E28" s="193" t="s">
         <v>190</v>
       </c>
-      <c r="F28" s="182"/>
+      <c r="F28" s="194"/>
       <c r="G28" s="65"/>
       <c r="H28" s="41"/>
       <c r="I28" s="28"/>
@@ -4344,10 +4525,10 @@
       <c r="S28" s="53"/>
       <c r="T28" s="41"/>
       <c r="V28" s="29"/>
-      <c r="W28" s="155"/>
-      <c r="X28" s="155"/>
-      <c r="Y28" s="155"/>
-      <c r="Z28" s="155"/>
+      <c r="W28" s="154"/>
+      <c r="X28" s="154"/>
+      <c r="Y28" s="154"/>
+      <c r="Z28" s="154"/>
       <c r="AA28" s="41"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.3">
@@ -4410,7 +4591,7 @@
       <c r="AA29" s="39"/>
     </row>
     <row r="30" spans="2:27" ht="33" x14ac:dyDescent="0.3">
-      <c r="B30" s="166">
+      <c r="B30" s="165">
         <v>15</v>
       </c>
       <c r="C30" s="42">
@@ -4458,20 +4639,20 @@
         <v>22</v>
       </c>
       <c r="X30" s="82" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Y30" s="82" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="Z30" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="AA30" s="164" t="s">
-        <v>477</v>
+      <c r="AA30" s="163" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B31" s="166">
+      <c r="B31" s="165">
         <v>16</v>
       </c>
       <c r="C31" s="42">
@@ -4519,16 +4700,16 @@
         <v>22</v>
       </c>
       <c r="X31" s="82" t="s">
+        <v>474</v>
+      </c>
+      <c r="Y31" s="82" t="s">
         <v>475</v>
-      </c>
-      <c r="Y31" s="82" t="s">
-        <v>476</v>
       </c>
       <c r="Z31" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="AA31" s="164" t="s">
-        <v>477</v>
+      <c r="AA31" s="163" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.3">
@@ -4600,10 +4781,10 @@
       <c r="D33" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="E33" s="181" t="s">
+      <c r="E33" s="193" t="s">
         <v>195</v>
       </c>
-      <c r="F33" s="182"/>
+      <c r="F33" s="194"/>
       <c r="G33" s="65"/>
       <c r="H33" s="41"/>
       <c r="I33" s="28"/>
@@ -4619,10 +4800,10 @@
       <c r="S33" s="53"/>
       <c r="T33" s="41"/>
       <c r="V33" s="29"/>
-      <c r="W33" s="155"/>
-      <c r="X33" s="155"/>
-      <c r="Y33" s="155"/>
-      <c r="Z33" s="155"/>
+      <c r="W33" s="154"/>
+      <c r="X33" s="154"/>
+      <c r="Y33" s="154"/>
+      <c r="Z33" s="154"/>
       <c r="AA33" s="41"/>
     </row>
     <row r="34" spans="2:28" x14ac:dyDescent="0.3">
@@ -4635,10 +4816,10 @@
       <c r="D34" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="E34" s="181" t="s">
+      <c r="E34" s="193" t="s">
         <v>176</v>
       </c>
-      <c r="F34" s="182"/>
+      <c r="F34" s="194"/>
       <c r="G34" s="65"/>
       <c r="H34" s="41"/>
       <c r="I34" s="28"/>
@@ -4654,14 +4835,14 @@
       <c r="S34" s="53"/>
       <c r="T34" s="41"/>
       <c r="V34" s="29"/>
-      <c r="W34" s="155"/>
-      <c r="X34" s="155"/>
-      <c r="Y34" s="155"/>
-      <c r="Z34" s="155"/>
+      <c r="W34" s="154"/>
+      <c r="X34" s="154"/>
+      <c r="Y34" s="154"/>
+      <c r="Z34" s="154"/>
       <c r="AA34" s="41"/>
     </row>
     <row r="35" spans="2:28" ht="33" x14ac:dyDescent="0.3">
-      <c r="B35" s="166">
+      <c r="B35" s="165">
         <v>20</v>
       </c>
       <c r="C35" s="13">
@@ -4714,8 +4895,8 @@
         <v>72</v>
       </c>
       <c r="T35" s="18"/>
-      <c r="V35" s="160" t="s">
-        <v>470</v>
+      <c r="V35" s="159" t="s">
+        <v>469</v>
       </c>
       <c r="W35" s="141" t="s">
         <v>379</v>
@@ -4732,7 +4913,7 @@
       <c r="AA35" s="134"/>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B36" s="166">
+      <c r="B36" s="165">
         <v>21</v>
       </c>
       <c r="C36" s="13">
@@ -4785,14 +4966,14 @@
         <v>72</v>
       </c>
       <c r="T36" s="18"/>
-      <c r="V36" s="160" t="s">
-        <v>471</v>
+      <c r="V36" s="159" t="s">
+        <v>470</v>
       </c>
       <c r="W36" s="141" t="s">
         <v>379</v>
       </c>
       <c r="X36" s="141" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="Y36" s="141" t="s">
         <v>72</v>
@@ -4803,7 +4984,7 @@
       <c r="AA36" s="134"/>
     </row>
     <row r="37" spans="2:28" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B37" s="166">
+      <c r="B37" s="165">
         <v>22</v>
       </c>
       <c r="C37" s="13">
@@ -4858,23 +5039,23 @@
         <v>25</v>
       </c>
       <c r="T37" s="139"/>
-      <c r="V37" s="161" t="s">
-        <v>472</v>
+      <c r="V37" s="160" t="s">
+        <v>471</v>
       </c>
       <c r="W37" s="141" t="s">
         <v>379</v>
       </c>
       <c r="X37" s="141" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="Y37" s="141" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="Z37" s="141" t="s">
         <v>72</v>
       </c>
-      <c r="AA37" s="165" t="s">
-        <v>478</v>
+      <c r="AA37" s="164" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="38" spans="2:28" ht="49.5" x14ac:dyDescent="0.3">
@@ -5022,7 +5203,7 @@
       <c r="C40" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D40" s="157" t="s">
+      <c r="D40" s="156" t="s">
         <v>48</v>
       </c>
       <c r="E40" s="13" t="s">
@@ -5096,7 +5277,7 @@
       <c r="C41" s="13">
         <v>18</v>
       </c>
-      <c r="D41" s="157" t="s">
+      <c r="D41" s="156" t="s">
         <v>38</v>
       </c>
       <c r="E41" s="11" t="s">
@@ -5167,7 +5348,7 @@
       <c r="C42" s="13">
         <v>19</v>
       </c>
-      <c r="D42" s="157" t="s">
+      <c r="D42" s="156" t="s">
         <v>42</v>
       </c>
       <c r="E42" s="11" t="s">
@@ -5456,10 +5637,10 @@
       <c r="D46" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="E46" s="181" t="s">
+      <c r="E46" s="193" t="s">
         <v>195</v>
       </c>
-      <c r="F46" s="182"/>
+      <c r="F46" s="194"/>
       <c r="G46" s="65"/>
       <c r="H46" s="41"/>
       <c r="I46" s="28"/>
@@ -5475,10 +5656,10 @@
       <c r="S46" s="53"/>
       <c r="T46" s="41"/>
       <c r="V46" s="29"/>
-      <c r="W46" s="155"/>
-      <c r="X46" s="155"/>
-      <c r="Y46" s="155"/>
-      <c r="Z46" s="155"/>
+      <c r="W46" s="154"/>
+      <c r="X46" s="154"/>
+      <c r="Y46" s="154"/>
+      <c r="Z46" s="154"/>
       <c r="AA46" s="41"/>
     </row>
     <row r="47" spans="2:28" x14ac:dyDescent="0.3">
@@ -5491,10 +5672,10 @@
       <c r="D47" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="E47" s="181" t="s">
+      <c r="E47" s="193" t="s">
         <v>176</v>
       </c>
-      <c r="F47" s="182"/>
+      <c r="F47" s="194"/>
       <c r="G47" s="65"/>
       <c r="H47" s="41"/>
       <c r="I47" s="28"/>
@@ -5510,10 +5691,10 @@
       <c r="S47" s="53"/>
       <c r="T47" s="41"/>
       <c r="V47" s="29"/>
-      <c r="W47" s="155"/>
-      <c r="X47" s="155"/>
-      <c r="Y47" s="155"/>
-      <c r="Z47" s="155"/>
+      <c r="W47" s="154"/>
+      <c r="X47" s="154"/>
+      <c r="Y47" s="154"/>
+      <c r="Z47" s="154"/>
       <c r="AA47" s="41"/>
     </row>
     <row r="48" spans="2:28" ht="49.5" x14ac:dyDescent="0.3">
@@ -5523,7 +5704,7 @@
       <c r="C48" s="13">
         <v>25</v>
       </c>
-      <c r="D48" s="157" t="s">
+      <c r="D48" s="156" t="s">
         <v>146</v>
       </c>
       <c r="E48" s="11" t="s">
@@ -5585,7 +5766,7 @@
       <c r="C49" s="13">
         <v>26</v>
       </c>
-      <c r="D49" s="157" t="s">
+      <c r="D49" s="156" t="s">
         <v>147</v>
       </c>
       <c r="E49" s="11" t="s">
@@ -5644,7 +5825,7 @@
       <c r="C50" s="13">
         <v>27</v>
       </c>
-      <c r="D50" s="157" t="s">
+      <c r="D50" s="156" t="s">
         <v>148</v>
       </c>
       <c r="E50" s="11" t="s">
@@ -5703,7 +5884,7 @@
       <c r="C51" s="13">
         <v>28</v>
       </c>
-      <c r="D51" s="157" t="s">
+      <c r="D51" s="156" t="s">
         <v>68</v>
       </c>
       <c r="E51" s="11" t="s">
@@ -5779,7 +5960,7 @@
       <c r="C52" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D52" s="157" t="s">
+      <c r="D52" s="156" t="s">
         <v>52</v>
       </c>
       <c r="E52" s="13" t="s">
@@ -5850,7 +6031,7 @@
       <c r="C53" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D53" s="157" t="s">
+      <c r="D53" s="156" t="s">
         <v>56</v>
       </c>
       <c r="E53" s="13" t="s">
@@ -6062,7 +6243,7 @@
       <c r="AA55" s="39"/>
     </row>
     <row r="56" spans="2:27" ht="33" x14ac:dyDescent="0.3">
-      <c r="B56" s="167">
+      <c r="B56" s="166">
         <v>41</v>
       </c>
       <c r="C56" s="13">
@@ -6074,7 +6255,7 @@
       <c r="E56" s="83" t="s">
         <v>282</v>
       </c>
-      <c r="F56" s="169" t="s">
+      <c r="F56" s="168" t="s">
         <v>181</v>
       </c>
       <c r="G56" s="64"/>
@@ -6253,7 +6434,7 @@
       <c r="AA58" s="94"/>
     </row>
     <row r="59" spans="2:27" ht="33" x14ac:dyDescent="0.3">
-      <c r="B59" s="167">
+      <c r="B59" s="166">
         <v>44</v>
       </c>
       <c r="C59" s="13">
@@ -6326,7 +6507,7 @@
       <c r="C60" s="13">
         <v>33</v>
       </c>
-      <c r="D60" s="157" t="s">
+      <c r="D60" s="156" t="s">
         <v>71</v>
       </c>
       <c r="E60" s="11" t="s">
@@ -6467,10 +6648,10 @@
       <c r="D62" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="E62" s="181" t="s">
+      <c r="E62" s="193" t="s">
         <v>195</v>
       </c>
-      <c r="F62" s="182"/>
+      <c r="F62" s="194"/>
       <c r="G62" s="65"/>
       <c r="H62" s="41"/>
       <c r="I62" s="28"/>
@@ -6486,10 +6667,10 @@
       <c r="S62" s="53"/>
       <c r="T62" s="41"/>
       <c r="V62" s="29"/>
-      <c r="W62" s="155"/>
-      <c r="X62" s="155"/>
-      <c r="Y62" s="155"/>
-      <c r="Z62" s="155"/>
+      <c r="W62" s="154"/>
+      <c r="X62" s="154"/>
+      <c r="Y62" s="154"/>
+      <c r="Z62" s="154"/>
       <c r="AA62" s="41"/>
     </row>
     <row r="63" spans="2:27" x14ac:dyDescent="0.3">
@@ -6502,10 +6683,10 @@
       <c r="D63" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="E63" s="181" t="s">
+      <c r="E63" s="193" t="s">
         <v>176</v>
       </c>
-      <c r="F63" s="182"/>
+      <c r="F63" s="194"/>
       <c r="G63" s="65"/>
       <c r="H63" s="41"/>
       <c r="I63" s="28"/>
@@ -6521,10 +6702,10 @@
       <c r="S63" s="53"/>
       <c r="T63" s="41"/>
       <c r="V63" s="29"/>
-      <c r="W63" s="155"/>
-      <c r="X63" s="155"/>
-      <c r="Y63" s="155"/>
-      <c r="Z63" s="155"/>
+      <c r="W63" s="154"/>
+      <c r="X63" s="154"/>
+      <c r="Y63" s="154"/>
+      <c r="Z63" s="154"/>
       <c r="AA63" s="41"/>
     </row>
     <row r="64" spans="2:27" x14ac:dyDescent="0.3">
@@ -6674,7 +6855,7 @@
       <c r="C66" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D66" s="157" t="s">
+      <c r="D66" s="156" t="s">
         <v>90</v>
       </c>
       <c r="E66" s="13" t="s">
@@ -6745,7 +6926,7 @@
       <c r="C67" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D67" s="157" t="s">
+      <c r="D67" s="156" t="s">
         <v>82</v>
       </c>
       <c r="E67" s="13" t="s">
@@ -6816,7 +6997,7 @@
       <c r="C68" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D68" s="163" t="s">
+      <c r="D68" s="162" t="s">
         <v>76</v>
       </c>
       <c r="E68" s="11" t="s">
@@ -7222,7 +7403,7 @@
       <c r="AA73" s="39"/>
     </row>
     <row r="74" spans="2:27" ht="33" x14ac:dyDescent="0.3">
-      <c r="B74" s="166">
+      <c r="B74" s="165">
         <v>59</v>
       </c>
       <c r="C74" s="13">
@@ -7278,7 +7459,7 @@
         <v>293</v>
       </c>
       <c r="X74" s="82" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="Y74" s="82" t="s">
         <v>264</v>
@@ -7298,10 +7479,10 @@
       <c r="D75" s="49" t="s">
         <v>225</v>
       </c>
-      <c r="E75" s="181" t="s">
+      <c r="E75" s="193" t="s">
         <v>244</v>
       </c>
-      <c r="F75" s="182"/>
+      <c r="F75" s="194"/>
       <c r="G75" s="65"/>
       <c r="H75" s="63"/>
       <c r="I75" s="29"/>
@@ -7323,16 +7504,16 @@
       <c r="V75" s="29" t="s">
         <v>295</v>
       </c>
-      <c r="W75" s="155"/>
-      <c r="X75" s="155" t="s">
+      <c r="W75" s="154"/>
+      <c r="X75" s="154" t="s">
         <v>295</v>
       </c>
-      <c r="Y75" s="155"/>
-      <c r="Z75" s="155"/>
+      <c r="Y75" s="154"/>
+      <c r="Z75" s="154"/>
       <c r="AA75" s="41"/>
     </row>
     <row r="76" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B76" s="166">
+      <c r="B76" s="165">
         <v>61</v>
       </c>
       <c r="C76" s="13">
@@ -7400,7 +7581,7 @@
         <v>305</v>
       </c>
       <c r="Y76" s="82" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Z76" s="82" t="s">
         <v>25</v>
@@ -7416,7 +7597,7 @@
       <c r="C77" s="13">
         <v>46</v>
       </c>
-      <c r="D77" s="157" t="s">
+      <c r="D77" s="156" t="s">
         <v>96</v>
       </c>
       <c r="E77" s="11" t="s">
@@ -7493,10 +7674,10 @@
       <c r="D78" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="E78" s="181" t="s">
+      <c r="E78" s="193" t="s">
         <v>195</v>
       </c>
-      <c r="F78" s="182"/>
+      <c r="F78" s="194"/>
       <c r="G78" s="65"/>
       <c r="H78" s="41"/>
       <c r="I78" s="28"/>
@@ -7512,10 +7693,10 @@
       <c r="S78" s="53"/>
       <c r="T78" s="41"/>
       <c r="V78" s="29"/>
-      <c r="W78" s="155"/>
-      <c r="X78" s="155"/>
-      <c r="Y78" s="155"/>
-      <c r="Z78" s="155"/>
+      <c r="W78" s="154"/>
+      <c r="X78" s="154"/>
+      <c r="Y78" s="154"/>
+      <c r="Z78" s="154"/>
       <c r="AA78" s="41"/>
     </row>
     <row r="79" spans="2:27" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -7528,10 +7709,10 @@
       <c r="D79" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="E79" s="183" t="s">
+      <c r="E79" s="195" t="s">
         <v>176</v>
       </c>
-      <c r="F79" s="184"/>
+      <c r="F79" s="196"/>
       <c r="G79" s="66"/>
       <c r="H79" s="68"/>
       <c r="I79" s="73"/>
@@ -7547,10 +7728,10 @@
       <c r="S79" s="54"/>
       <c r="T79" s="68"/>
       <c r="V79" s="30"/>
-      <c r="W79" s="156"/>
-      <c r="X79" s="156"/>
-      <c r="Y79" s="156"/>
-      <c r="Z79" s="156"/>
+      <c r="W79" s="155"/>
+      <c r="X79" s="155"/>
+      <c r="Y79" s="155"/>
+      <c r="Z79" s="155"/>
       <c r="AA79" s="68"/>
     </row>
     <row r="84" spans="5:6" x14ac:dyDescent="0.3">
@@ -7604,18 +7785,6 @@
   </sheetData>
   <autoFilter ref="B15:AB79"/>
   <mergeCells count="28">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="G14:H14"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="O14:P14"/>
     <mergeCell ref="X14:AA14"/>
@@ -7632,6 +7801,18 @@
     <mergeCell ref="E62:F62"/>
     <mergeCell ref="E63:F63"/>
     <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8286,10 +8467,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N46"/>
+  <dimension ref="B2:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="P28" sqref="P28:P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8298,1051 +8479,1350 @@
     <col min="3" max="3" width="12.75" style="143" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.625" style="143" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.625" style="143" customWidth="1"/>
-    <col min="6" max="6" width="9" style="144"/>
-    <col min="7" max="7" width="11.875" style="143" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.375" style="143" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" style="143" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="143" customWidth="1"/>
+    <col min="8" max="8" width="9" style="144"/>
+    <col min="9" max="9" width="11.875" style="143" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.375" style="143" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.625" style="143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="144" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="3" spans="2:14" s="144" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="145" t="s">
-        <v>459</v>
-      </c>
-      <c r="C3" s="118" t="s">
+    <row r="3" spans="2:16" s="144" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="197" t="s">
+        <v>458</v>
+      </c>
+      <c r="C3" s="198" t="s">
         <v>442</v>
       </c>
-      <c r="D3" s="118" t="s">
-        <v>443</v>
-      </c>
-      <c r="E3" s="119" t="s">
-        <v>464</v>
-      </c>
-      <c r="F3" s="145" t="s">
-        <v>459</v>
-      </c>
-      <c r="G3" s="118" t="s">
+      <c r="D3" s="198" t="s">
+        <v>481</v>
+      </c>
+      <c r="E3" s="198" t="s">
+        <v>463</v>
+      </c>
+      <c r="F3" s="199" t="s">
+        <v>482</v>
+      </c>
+      <c r="G3" s="200" t="s">
+        <v>463</v>
+      </c>
+      <c r="H3" s="197" t="s">
+        <v>458</v>
+      </c>
+      <c r="I3" s="198" t="s">
         <v>442</v>
       </c>
-      <c r="H3" s="118" t="s">
-        <v>443</v>
-      </c>
-      <c r="I3" s="119" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="153">
+      <c r="J3" s="198" t="s">
+        <v>481</v>
+      </c>
+      <c r="K3" s="198" t="s">
+        <v>463</v>
+      </c>
+      <c r="L3" s="199" t="s">
+        <v>482</v>
+      </c>
+      <c r="M3" s="200" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="152">
         <v>1</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="150" t="s">
         <v>384</v>
       </c>
-      <c r="D4" s="146" t="s">
+      <c r="D4" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G4" s="146"/>
+      <c r="H4" s="152">
+        <v>2</v>
+      </c>
+      <c r="I4" s="150" t="s">
+        <v>385</v>
+      </c>
+      <c r="J4" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K4" s="114"/>
+      <c r="L4" s="145" t="s">
+        <v>489</v>
+      </c>
+      <c r="M4" s="146" t="s">
+        <v>490</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="152">
+        <v>3</v>
+      </c>
+      <c r="C5" s="150" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5" s="150" t="s">
         <v>444</v>
       </c>
-      <c r="E4" s="147"/>
-      <c r="F4" s="153">
-        <v>2</v>
-      </c>
-      <c r="G4" s="151" t="s">
-        <v>385</v>
-      </c>
-      <c r="H4" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I4" s="115"/>
-      <c r="M4" s="5">
+      <c r="E5" s="150" t="s">
+        <v>453</v>
+      </c>
+      <c r="F5" s="150" t="s">
+        <v>483</v>
+      </c>
+      <c r="G5" s="149"/>
+      <c r="H5" s="152">
+        <v>4</v>
+      </c>
+      <c r="I5" s="150" t="s">
+        <v>387</v>
+      </c>
+      <c r="J5" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K5" s="114"/>
+      <c r="L5" s="150" t="s">
+        <v>491</v>
+      </c>
+      <c r="M5" s="149"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="152">
+        <v>5</v>
+      </c>
+      <c r="C6" s="150" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6" s="150" t="s">
+        <v>445</v>
+      </c>
+      <c r="E6" s="150"/>
+      <c r="F6" s="150" t="s">
+        <v>484</v>
+      </c>
+      <c r="G6" s="149"/>
+      <c r="H6" s="152">
+        <v>6</v>
+      </c>
+      <c r="I6" s="150" t="s">
+        <v>389</v>
+      </c>
+      <c r="J6" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K6" s="114"/>
+      <c r="L6" s="150" t="s">
+        <v>492</v>
+      </c>
+      <c r="M6" s="149"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="152">
+        <v>7</v>
+      </c>
+      <c r="C7" s="150" t="s">
+        <v>390</v>
+      </c>
+      <c r="D7" s="150" t="s">
+        <v>446</v>
+      </c>
+      <c r="E7" s="150"/>
+      <c r="F7" s="150" t="s">
+        <v>485</v>
+      </c>
+      <c r="G7" s="149"/>
+      <c r="H7" s="152">
+        <v>8</v>
+      </c>
+      <c r="I7" s="150" t="s">
+        <v>392</v>
+      </c>
+      <c r="J7" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K7" s="114"/>
+      <c r="L7" s="150" t="s">
+        <v>493</v>
+      </c>
+      <c r="M7" s="149"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="152">
+        <v>9</v>
+      </c>
+      <c r="C8" s="150" t="s">
+        <v>391</v>
+      </c>
+      <c r="D8" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E8" s="145"/>
+      <c r="F8" s="145" t="s">
+        <v>486</v>
+      </c>
+      <c r="G8" s="146"/>
+      <c r="H8" s="152">
+        <v>10</v>
+      </c>
+      <c r="I8" s="150" t="s">
+        <v>393</v>
+      </c>
+      <c r="J8" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K8" s="114"/>
+      <c r="L8" s="145" t="s">
+        <v>494</v>
+      </c>
+      <c r="M8" s="146"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="152">
+        <v>11</v>
+      </c>
+      <c r="C9" s="150" t="s">
+        <v>394</v>
+      </c>
+      <c r="D9" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E9" s="145"/>
+      <c r="F9" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G9" s="146"/>
+      <c r="H9" s="152">
+        <v>12</v>
+      </c>
+      <c r="I9" s="150" t="s">
+        <v>395</v>
+      </c>
+      <c r="J9" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K9" s="114"/>
+      <c r="L9" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M9" s="146"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="152">
+        <v>13</v>
+      </c>
+      <c r="C10" s="150" t="s">
+        <v>396</v>
+      </c>
+      <c r="D10" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E10" s="145"/>
+      <c r="F10" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G10" s="146"/>
+      <c r="H10" s="152">
+        <v>14</v>
+      </c>
+      <c r="I10" s="150" t="s">
+        <v>397</v>
+      </c>
+      <c r="J10" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K10" s="114"/>
+      <c r="L10" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M10" s="146"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="152">
+        <v>15</v>
+      </c>
+      <c r="C11" s="150" t="s">
+        <v>398</v>
+      </c>
+      <c r="D11" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E11" s="145"/>
+      <c r="F11" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G11" s="146"/>
+      <c r="H11" s="152">
+        <v>16</v>
+      </c>
+      <c r="I11" s="150" t="s">
+        <v>400</v>
+      </c>
+      <c r="J11" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K11" s="114"/>
+      <c r="L11" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M11" s="146"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="152">
+        <v>17</v>
+      </c>
+      <c r="C12" s="150" t="s">
+        <v>399</v>
+      </c>
+      <c r="D12" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E12" s="145"/>
+      <c r="F12" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G12" s="146"/>
+      <c r="H12" s="152">
+        <v>18</v>
+      </c>
+      <c r="I12" s="150" t="s">
+        <v>401</v>
+      </c>
+      <c r="J12" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K12" s="114"/>
+      <c r="L12" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M12" s="146"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="152">
+        <v>19</v>
+      </c>
+      <c r="C13" s="150" t="s">
+        <v>402</v>
+      </c>
+      <c r="D13" s="150" t="s">
+        <v>402</v>
+      </c>
+      <c r="E13" s="150"/>
+      <c r="F13" s="150" t="s">
+        <v>402</v>
+      </c>
+      <c r="G13" s="149"/>
+      <c r="H13" s="152">
+        <v>20</v>
+      </c>
+      <c r="I13" s="150" t="s">
+        <v>403</v>
+      </c>
+      <c r="J13" s="150" t="s">
+        <v>403</v>
+      </c>
+      <c r="K13" s="114"/>
+      <c r="L13" s="150" t="s">
+        <v>403</v>
+      </c>
+      <c r="M13" s="149"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="152">
+        <v>21</v>
+      </c>
+      <c r="C14" s="150" t="s">
+        <v>404</v>
+      </c>
+      <c r="D14" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E14" s="150"/>
+      <c r="F14" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G14" s="149"/>
+      <c r="H14" s="152">
+        <v>22</v>
+      </c>
+      <c r="I14" s="150" t="s">
+        <v>405</v>
+      </c>
+      <c r="J14" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K14" s="114"/>
+      <c r="L14" s="145" t="s">
+        <v>495</v>
+      </c>
+      <c r="M14" s="149"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="152">
+        <v>23</v>
+      </c>
+      <c r="C15" s="150" t="s">
+        <v>406</v>
+      </c>
+      <c r="D15" s="150" t="s">
+        <v>447</v>
+      </c>
+      <c r="E15" s="150"/>
+      <c r="F15" s="150" t="s">
+        <v>447</v>
+      </c>
+      <c r="G15" s="149"/>
+      <c r="H15" s="152">
+        <v>24</v>
+      </c>
+      <c r="I15" s="150" t="s">
+        <v>406</v>
+      </c>
+      <c r="J15" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K15" s="114"/>
+      <c r="L15" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M15" s="149"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="152">
+        <v>25</v>
+      </c>
+      <c r="C16" s="150" t="s">
+        <v>407</v>
+      </c>
+      <c r="D16" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E16" s="145"/>
+      <c r="F16" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G16" s="146"/>
+      <c r="H16" s="152">
+        <v>26</v>
+      </c>
+      <c r="I16" s="150" t="s">
+        <v>414</v>
+      </c>
+      <c r="J16" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K16" s="114"/>
+      <c r="L16" s="145" t="s">
+        <v>496</v>
+      </c>
+      <c r="M16" s="146"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="152">
+        <v>27</v>
+      </c>
+      <c r="C17" s="150" t="s">
+        <v>408</v>
+      </c>
+      <c r="D17" s="150" t="s">
+        <v>447</v>
+      </c>
+      <c r="E17" s="145"/>
+      <c r="F17" s="150" t="s">
+        <v>447</v>
+      </c>
+      <c r="G17" s="146"/>
+      <c r="H17" s="152">
+        <v>28</v>
+      </c>
+      <c r="I17" s="150" t="s">
+        <v>415</v>
+      </c>
+      <c r="J17" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K17" s="114"/>
+      <c r="L17" s="150" t="s">
+        <v>497</v>
+      </c>
+      <c r="M17" s="146"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="152">
+        <v>29</v>
+      </c>
+      <c r="C18" s="150" t="s">
+        <v>409</v>
+      </c>
+      <c r="D18" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E18" s="145"/>
+      <c r="F18" s="145" t="s">
+        <v>487</v>
+      </c>
+      <c r="G18" s="146"/>
+      <c r="H18" s="152">
+        <v>30</v>
+      </c>
+      <c r="I18" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="J18" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K18" s="114"/>
+      <c r="L18" s="145" t="s">
+        <v>498</v>
+      </c>
+      <c r="M18" s="146"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="152">
+        <v>31</v>
+      </c>
+      <c r="C19" s="150" t="s">
+        <v>410</v>
+      </c>
+      <c r="D19" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E19" s="145"/>
+      <c r="F19" s="145" t="s">
+        <v>488</v>
+      </c>
+      <c r="G19" s="146"/>
+      <c r="H19" s="152">
+        <v>32</v>
+      </c>
+      <c r="I19" s="150" t="s">
+        <v>417</v>
+      </c>
+      <c r="J19" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K19" s="114"/>
+      <c r="L19" s="145" t="s">
+        <v>499</v>
+      </c>
+      <c r="M19" s="146"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20" s="152">
+        <v>33</v>
+      </c>
+      <c r="C20" s="150" t="s">
+        <v>411</v>
+      </c>
+      <c r="D20" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E20" s="145"/>
+      <c r="F20" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G20" s="146"/>
+      <c r="H20" s="152">
+        <v>34</v>
+      </c>
+      <c r="I20" s="150" t="s">
+        <v>418</v>
+      </c>
+      <c r="J20" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K20" s="114"/>
+      <c r="L20" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M20" s="146"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21" s="152">
+        <v>35</v>
+      </c>
+      <c r="C21" s="150" t="s">
+        <v>412</v>
+      </c>
+      <c r="D21" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E21" s="145"/>
+      <c r="F21" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G21" s="146"/>
+      <c r="H21" s="152">
+        <v>36</v>
+      </c>
+      <c r="I21" s="150" t="s">
+        <v>419</v>
+      </c>
+      <c r="J21" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K21" s="114"/>
+      <c r="L21" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M21" s="146"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="152">
+        <v>37</v>
+      </c>
+      <c r="C22" s="150" t="s">
+        <v>413</v>
+      </c>
+      <c r="D22" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E22" s="145"/>
+      <c r="F22" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G22" s="146"/>
+      <c r="H22" s="152">
+        <v>38</v>
+      </c>
+      <c r="I22" s="150" t="s">
+        <v>420</v>
+      </c>
+      <c r="J22" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K22" s="114"/>
+      <c r="L22" s="145" t="s">
+        <v>500</v>
+      </c>
+      <c r="M22" s="146"/>
+    </row>
+    <row r="23" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="153">
         <v>39</v>
       </c>
-      <c r="N4" s="5">
-        <v>32.42</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="153">
-        <v>3</v>
-      </c>
-      <c r="C5" s="151" t="s">
-        <v>386</v>
-      </c>
-      <c r="D5" s="151" t="s">
-        <v>445</v>
-      </c>
-      <c r="E5" s="150" t="s">
-        <v>454</v>
-      </c>
-      <c r="F5" s="153">
-        <v>4</v>
-      </c>
-      <c r="G5" s="151" t="s">
-        <v>387</v>
-      </c>
-      <c r="H5" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I5" s="115"/>
-      <c r="M5" s="5">
-        <v>32.42</v>
-      </c>
-      <c r="N5" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="153">
-        <v>5</v>
-      </c>
-      <c r="C6" s="151" t="s">
-        <v>388</v>
-      </c>
-      <c r="D6" s="151" t="s">
-        <v>446</v>
-      </c>
-      <c r="E6" s="150"/>
-      <c r="F6" s="153">
-        <v>6</v>
-      </c>
-      <c r="G6" s="151" t="s">
-        <v>389</v>
-      </c>
-      <c r="H6" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I6" s="115"/>
-      <c r="M6" s="5">
-        <f>M4-M5</f>
-        <v>6.5799999999999983</v>
-      </c>
-      <c r="N6" s="5">
-        <f>N4+N5</f>
-        <v>36.42</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="153">
-        <v>7</v>
-      </c>
-      <c r="C7" s="151" t="s">
-        <v>390</v>
-      </c>
-      <c r="D7" s="151" t="s">
-        <v>447</v>
-      </c>
-      <c r="E7" s="150"/>
-      <c r="F7" s="153">
-        <v>8</v>
-      </c>
-      <c r="G7" s="151" t="s">
-        <v>392</v>
-      </c>
-      <c r="H7" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I7" s="115"/>
-      <c r="M7" s="5">
-        <v>2</v>
-      </c>
-      <c r="N7" s="5">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="153">
-        <v>9</v>
-      </c>
-      <c r="C8" s="151" t="s">
-        <v>391</v>
-      </c>
-      <c r="D8" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E8" s="147"/>
-      <c r="F8" s="153">
-        <v>10</v>
-      </c>
-      <c r="G8" s="151" t="s">
-        <v>393</v>
-      </c>
-      <c r="H8" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I8" s="115"/>
-      <c r="M8" s="5">
-        <f>M6-M7</f>
-        <v>4.5799999999999983</v>
-      </c>
-      <c r="N8" s="5">
-        <f>N7-N6</f>
-        <v>2.5799999999999983</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="153">
-        <v>11</v>
-      </c>
-      <c r="C9" s="151" t="s">
-        <v>394</v>
-      </c>
-      <c r="D9" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E9" s="147"/>
-      <c r="F9" s="153">
-        <v>12</v>
-      </c>
-      <c r="G9" s="151" t="s">
-        <v>395</v>
-      </c>
-      <c r="H9" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I9" s="115"/>
-      <c r="M9" s="5">
-        <v>2</v>
-      </c>
-      <c r="N9" s="5">
-        <f>N8/2</f>
-        <v>1.2899999999999991</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="153">
-        <v>13</v>
-      </c>
-      <c r="C10" s="151" t="s">
-        <v>396</v>
-      </c>
-      <c r="D10" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E10" s="147"/>
-      <c r="F10" s="153">
-        <v>14</v>
-      </c>
-      <c r="G10" s="151" t="s">
-        <v>397</v>
-      </c>
-      <c r="H10" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I10" s="115"/>
-      <c r="M10" s="5">
-        <f>M8-M9</f>
-        <v>2.5799999999999983</v>
-      </c>
-      <c r="N10" s="5"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="153">
-        <v>15</v>
-      </c>
-      <c r="C11" s="151" t="s">
-        <v>398</v>
-      </c>
-      <c r="D11" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E11" s="147"/>
-      <c r="F11" s="153">
-        <v>16</v>
-      </c>
-      <c r="G11" s="151" t="s">
-        <v>400</v>
-      </c>
-      <c r="H11" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I11" s="115"/>
-      <c r="M11" s="5">
-        <f>M10/2</f>
-        <v>1.2899999999999991</v>
-      </c>
-      <c r="N11" s="5"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="153">
-        <v>17</v>
-      </c>
-      <c r="C12" s="151" t="s">
-        <v>399</v>
-      </c>
-      <c r="D12" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E12" s="147"/>
-      <c r="F12" s="153">
-        <v>18</v>
-      </c>
-      <c r="G12" s="151" t="s">
-        <v>401</v>
-      </c>
-      <c r="H12" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I12" s="115"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="153">
-        <v>19</v>
-      </c>
-      <c r="C13" s="151" t="s">
-        <v>402</v>
-      </c>
-      <c r="D13" s="151" t="s">
-        <v>402</v>
-      </c>
-      <c r="E13" s="150"/>
-      <c r="F13" s="153">
-        <v>20</v>
-      </c>
-      <c r="G13" s="151" t="s">
-        <v>403</v>
-      </c>
-      <c r="H13" s="151" t="s">
-        <v>403</v>
-      </c>
-      <c r="I13" s="115"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="153">
-        <v>21</v>
-      </c>
-      <c r="C14" s="151" t="s">
-        <v>404</v>
-      </c>
-      <c r="D14" s="151" t="s">
-        <v>448</v>
-      </c>
-      <c r="E14" s="150"/>
-      <c r="F14" s="153">
-        <v>22</v>
-      </c>
-      <c r="G14" s="151" t="s">
-        <v>405</v>
-      </c>
-      <c r="H14" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I14" s="115"/>
-      <c r="M14" s="5">
-        <v>2.58</v>
-      </c>
-      <c r="N14" s="5"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="153">
-        <v>23</v>
-      </c>
-      <c r="C15" s="151" t="s">
-        <v>406</v>
-      </c>
-      <c r="D15" s="151" t="s">
-        <v>448</v>
-      </c>
-      <c r="E15" s="150"/>
-      <c r="F15" s="153">
-        <v>24</v>
-      </c>
-      <c r="G15" s="151" t="s">
-        <v>406</v>
-      </c>
-      <c r="H15" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I15" s="115"/>
-      <c r="M15" s="5">
-        <v>2</v>
-      </c>
-      <c r="N15" s="5"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="153">
-        <v>25</v>
-      </c>
-      <c r="C16" s="151" t="s">
-        <v>407</v>
-      </c>
-      <c r="D16" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E16" s="147"/>
-      <c r="F16" s="153">
-        <v>26</v>
-      </c>
-      <c r="G16" s="151" t="s">
-        <v>414</v>
-      </c>
-      <c r="H16" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I16" s="115"/>
-      <c r="M16" s="5">
-        <f>M14+M15</f>
-        <v>4.58</v>
-      </c>
-      <c r="N16" s="5"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="153">
-        <v>27</v>
-      </c>
-      <c r="C17" s="151" t="s">
+      <c r="C23" s="151" t="s">
         <v>408</v>
       </c>
-      <c r="D17" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E17" s="147"/>
-      <c r="F17" s="153">
-        <v>28</v>
-      </c>
-      <c r="G17" s="151" t="s">
+      <c r="D23" s="147" t="s">
+        <v>443</v>
+      </c>
+      <c r="E23" s="147"/>
+      <c r="F23" s="147" t="s">
+        <v>443</v>
+      </c>
+      <c r="G23" s="148"/>
+      <c r="H23" s="153">
+        <v>40</v>
+      </c>
+      <c r="I23" s="151" t="s">
         <v>415</v>
       </c>
-      <c r="H17" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I17" s="115"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="153">
-        <v>29</v>
-      </c>
-      <c r="C18" s="151" t="s">
-        <v>409</v>
-      </c>
-      <c r="D18" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E18" s="147"/>
-      <c r="F18" s="153">
-        <v>30</v>
-      </c>
-      <c r="G18" s="151" t="s">
-        <v>416</v>
-      </c>
-      <c r="H18" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I18" s="115"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="153">
-        <v>31</v>
-      </c>
-      <c r="C19" s="151" t="s">
-        <v>410</v>
-      </c>
-      <c r="D19" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E19" s="147"/>
-      <c r="F19" s="153">
-        <v>32</v>
-      </c>
-      <c r="G19" s="151" t="s">
-        <v>417</v>
-      </c>
-      <c r="H19" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I19" s="115"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="153">
-        <v>33</v>
-      </c>
-      <c r="C20" s="151" t="s">
-        <v>411</v>
-      </c>
-      <c r="D20" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E20" s="147"/>
-      <c r="F20" s="153">
-        <v>34</v>
-      </c>
-      <c r="G20" s="151" t="s">
-        <v>418</v>
-      </c>
-      <c r="H20" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I20" s="115"/>
-      <c r="M20" s="5">
-        <v>2</v>
-      </c>
-      <c r="N20" s="5"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="153">
-        <v>35</v>
-      </c>
-      <c r="C21" s="151" t="s">
-        <v>412</v>
-      </c>
-      <c r="D21" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E21" s="147"/>
-      <c r="F21" s="153">
-        <v>36</v>
-      </c>
-      <c r="G21" s="151" t="s">
-        <v>419</v>
-      </c>
-      <c r="H21" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I21" s="115"/>
-      <c r="M21" s="5">
-        <v>19</v>
-      </c>
-      <c r="N21" s="5"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="153">
-        <v>37</v>
-      </c>
-      <c r="C22" s="151" t="s">
-        <v>413</v>
-      </c>
-      <c r="D22" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E22" s="147"/>
-      <c r="F22" s="153">
-        <v>38</v>
-      </c>
-      <c r="G22" s="151" t="s">
-        <v>420</v>
-      </c>
-      <c r="H22" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I22" s="115"/>
-      <c r="M22">
-        <f>M20*M21</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="154">
-        <v>39</v>
-      </c>
-      <c r="C23" s="152" t="s">
-        <v>408</v>
-      </c>
-      <c r="D23" s="148" t="s">
-        <v>444</v>
-      </c>
-      <c r="E23" s="149"/>
-      <c r="F23" s="154">
-        <v>40</v>
-      </c>
-      <c r="G23" s="152" t="s">
-        <v>415</v>
-      </c>
-      <c r="H23" s="148" t="s">
-        <v>444</v>
-      </c>
-      <c r="I23" s="117"/>
-    </row>
-    <row r="25" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J23" s="147" t="s">
+        <v>443</v>
+      </c>
+      <c r="K23" s="116"/>
+      <c r="L23" s="147" t="s">
+        <v>443</v>
+      </c>
+      <c r="M23" s="148"/>
+    </row>
+    <row r="25" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="144" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="26" spans="2:14" s="144" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="145" t="s">
+    <row r="26" spans="2:16" s="144" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="197" t="s">
+        <v>458</v>
+      </c>
+      <c r="C26" s="198" t="s">
+        <v>442</v>
+      </c>
+      <c r="D26" s="198" t="s">
+        <v>481</v>
+      </c>
+      <c r="E26" s="198" t="s">
+        <v>463</v>
+      </c>
+      <c r="F26" s="199" t="s">
+        <v>482</v>
+      </c>
+      <c r="G26" s="200" t="s">
+        <v>463</v>
+      </c>
+      <c r="H26" s="197" t="s">
+        <v>458</v>
+      </c>
+      <c r="I26" s="198" t="s">
+        <v>442</v>
+      </c>
+      <c r="J26" s="198" t="s">
+        <v>481</v>
+      </c>
+      <c r="K26" s="198" t="s">
+        <v>463</v>
+      </c>
+      <c r="L26" s="199" t="s">
+        <v>482</v>
+      </c>
+      <c r="M26" s="200" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B27" s="152">
+        <v>1</v>
+      </c>
+      <c r="C27" s="150" t="s">
+        <v>454</v>
+      </c>
+      <c r="D27" s="150" t="s">
+        <v>448</v>
+      </c>
+      <c r="E27" s="150" t="s">
         <v>459</v>
       </c>
-      <c r="C26" s="118" t="s">
-        <v>442</v>
-      </c>
-      <c r="D26" s="118" t="s">
-        <v>443</v>
-      </c>
-      <c r="E26" s="119" t="s">
-        <v>464</v>
-      </c>
-      <c r="F26" s="145" t="s">
-        <v>459</v>
-      </c>
-      <c r="G26" s="118" t="s">
-        <v>442</v>
-      </c>
-      <c r="H26" s="118" t="s">
-        <v>443</v>
-      </c>
-      <c r="I26" s="119" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="153">
-        <v>1</v>
-      </c>
-      <c r="C27" s="151" t="s">
+      <c r="F27" s="150" t="s">
+        <v>501</v>
+      </c>
+      <c r="G27" s="149"/>
+      <c r="H27" s="152">
+        <v>2</v>
+      </c>
+      <c r="I27" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="J27" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K27" s="114"/>
+      <c r="L27" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M27" s="149"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B28" s="152">
+        <v>3</v>
+      </c>
+      <c r="C28" s="150" t="s">
+        <v>425</v>
+      </c>
+      <c r="D28" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145" t="s">
+        <v>502</v>
+      </c>
+      <c r="G28" s="146"/>
+      <c r="H28" s="152">
+        <v>4</v>
+      </c>
+      <c r="I28" s="150" t="s">
+        <v>427</v>
+      </c>
+      <c r="J28" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K28" s="114"/>
+      <c r="L28" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M28" s="146"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B29" s="152">
+        <v>5</v>
+      </c>
+      <c r="C29" s="150" t="s">
+        <v>423</v>
+      </c>
+      <c r="D29" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E29" s="145"/>
+      <c r="F29" s="145" t="s">
+        <v>503</v>
+      </c>
+      <c r="G29" s="146"/>
+      <c r="H29" s="152">
+        <v>6</v>
+      </c>
+      <c r="I29" s="150" t="s">
+        <v>428</v>
+      </c>
+      <c r="J29" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K29" s="114"/>
+      <c r="L29" s="145" t="s">
+        <v>517</v>
+      </c>
+      <c r="M29" s="146"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="152">
+        <v>7</v>
+      </c>
+      <c r="C30" s="150" t="s">
+        <v>424</v>
+      </c>
+      <c r="D30" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G30" s="146"/>
+      <c r="H30" s="152">
+        <v>8</v>
+      </c>
+      <c r="I30" s="150" t="s">
+        <v>425</v>
+      </c>
+      <c r="J30" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K30" s="114"/>
+      <c r="L30" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M30" s="146"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31" s="152">
+        <v>9</v>
+      </c>
+      <c r="C31" s="150" t="s">
+        <v>404</v>
+      </c>
+      <c r="D31" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E31" s="145"/>
+      <c r="F31" s="145" t="s">
+        <v>504</v>
+      </c>
+      <c r="G31" s="146"/>
+      <c r="H31" s="152">
+        <v>10</v>
+      </c>
+      <c r="I31" s="150" t="s">
+        <v>405</v>
+      </c>
+      <c r="J31" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K31" s="114"/>
+      <c r="L31" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M31" s="146"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32" s="152">
+        <v>11</v>
+      </c>
+      <c r="C32" s="150" t="s">
+        <v>429</v>
+      </c>
+      <c r="D32" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E32" s="145"/>
+      <c r="F32" s="145" t="s">
+        <v>505</v>
+      </c>
+      <c r="G32" s="146"/>
+      <c r="H32" s="152">
+        <v>12</v>
+      </c>
+      <c r="I32" s="150" t="s">
+        <v>438</v>
+      </c>
+      <c r="J32" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K32" s="114"/>
+      <c r="L32" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M32" s="146"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B33" s="152">
+        <v>13</v>
+      </c>
+      <c r="C33" s="150" t="s">
         <v>455</v>
       </c>
-      <c r="D27" s="151" t="s">
+      <c r="D33" s="150" t="s">
         <v>449</v>
       </c>
-      <c r="E27" s="150" t="s">
+      <c r="E33" s="150" t="s">
         <v>460</v>
       </c>
-      <c r="F27" s="153">
-        <v>2</v>
-      </c>
-      <c r="G27" s="151" t="s">
-        <v>426</v>
-      </c>
-      <c r="H27" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I27" s="115"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="153">
-        <v>3</v>
-      </c>
-      <c r="C28" s="151" t="s">
-        <v>425</v>
-      </c>
-      <c r="D28" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E28" s="147"/>
-      <c r="F28" s="153">
-        <v>4</v>
-      </c>
-      <c r="G28" s="151" t="s">
+      <c r="F33" s="150" t="s">
+        <v>506</v>
+      </c>
+      <c r="G33" s="149"/>
+      <c r="H33" s="152">
+        <v>14</v>
+      </c>
+      <c r="I33" s="150" t="s">
+        <v>411</v>
+      </c>
+      <c r="J33" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K33" s="114"/>
+      <c r="L33" s="150" t="s">
+        <v>520</v>
+      </c>
+      <c r="M33" s="149"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B34" s="152">
+        <v>15</v>
+      </c>
+      <c r="C34" s="150" t="s">
+        <v>418</v>
+      </c>
+      <c r="D34" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E34" s="145"/>
+      <c r="F34" s="145" t="s">
+        <v>507</v>
+      </c>
+      <c r="G34" s="146"/>
+      <c r="H34" s="152">
+        <v>16</v>
+      </c>
+      <c r="I34" s="150" t="s">
+        <v>412</v>
+      </c>
+      <c r="J34" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K34" s="114"/>
+      <c r="L34" s="145" t="s">
+        <v>521</v>
+      </c>
+      <c r="M34" s="146"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B35" s="152">
+        <v>17</v>
+      </c>
+      <c r="C35" s="150" t="s">
         <v>427</v>
       </c>
-      <c r="H28" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I28" s="115"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="153">
-        <v>5</v>
-      </c>
-      <c r="C29" s="151" t="s">
+      <c r="D35" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E35" s="145"/>
+      <c r="F35" s="145" t="s">
+        <v>508</v>
+      </c>
+      <c r="G35" s="146"/>
+      <c r="H35" s="152">
+        <v>18</v>
+      </c>
+      <c r="I35" s="150" t="s">
+        <v>428</v>
+      </c>
+      <c r="J35" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K35" s="114"/>
+      <c r="L35" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M35" s="146"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B36" s="152">
+        <v>19</v>
+      </c>
+      <c r="C36" s="150" t="s">
+        <v>430</v>
+      </c>
+      <c r="D36" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E36" s="145"/>
+      <c r="F36" s="145" t="s">
+        <v>509</v>
+      </c>
+      <c r="G36" s="146"/>
+      <c r="H36" s="152">
+        <v>20</v>
+      </c>
+      <c r="I36" s="150" t="s">
+        <v>435</v>
+      </c>
+      <c r="J36" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K36" s="114"/>
+      <c r="L36" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M36" s="146"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B37" s="152">
+        <v>21</v>
+      </c>
+      <c r="C37" s="150" t="s">
+        <v>431</v>
+      </c>
+      <c r="D37" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E37" s="145"/>
+      <c r="F37" s="145" t="s">
+        <v>510</v>
+      </c>
+      <c r="G37" s="146"/>
+      <c r="H37" s="152">
+        <v>22</v>
+      </c>
+      <c r="I37" s="150" t="s">
+        <v>456</v>
+      </c>
+      <c r="J37" s="150" t="s">
+        <v>461</v>
+      </c>
+      <c r="K37" s="150" t="s">
+        <v>450</v>
+      </c>
+      <c r="L37" s="145" t="s">
+        <v>518</v>
+      </c>
+      <c r="M37" s="146"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B38" s="152">
+        <v>23</v>
+      </c>
+      <c r="C38" s="150" t="s">
+        <v>432</v>
+      </c>
+      <c r="D38" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E38" s="145"/>
+      <c r="F38" s="145" t="s">
+        <v>511</v>
+      </c>
+      <c r="G38" s="146"/>
+      <c r="H38" s="152">
+        <v>24</v>
+      </c>
+      <c r="I38" s="150" t="s">
+        <v>457</v>
+      </c>
+      <c r="J38" s="150" t="s">
+        <v>462</v>
+      </c>
+      <c r="K38" s="150" t="s">
+        <v>451</v>
+      </c>
+      <c r="L38" s="145" t="s">
+        <v>519</v>
+      </c>
+      <c r="M38" s="146"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B39" s="152">
+        <v>25</v>
+      </c>
+      <c r="C39" s="150" t="s">
+        <v>430</v>
+      </c>
+      <c r="D39" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E39" s="145"/>
+      <c r="F39" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G39" s="146"/>
+      <c r="H39" s="152">
+        <v>26</v>
+      </c>
+      <c r="I39" s="150" t="s">
+        <v>431</v>
+      </c>
+      <c r="J39" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K39" s="114"/>
+      <c r="L39" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M39" s="146"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B40" s="152">
+        <v>27</v>
+      </c>
+      <c r="C40" s="150" t="s">
+        <v>433</v>
+      </c>
+      <c r="D40" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E40" s="145"/>
+      <c r="F40" s="145" t="s">
+        <v>512</v>
+      </c>
+      <c r="G40" s="146"/>
+      <c r="H40" s="152">
+        <v>28</v>
+      </c>
+      <c r="I40" s="150" t="s">
+        <v>439</v>
+      </c>
+      <c r="J40" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K40" s="114"/>
+      <c r="L40" s="145" t="s">
+        <v>522</v>
+      </c>
+      <c r="M40" s="146"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B41" s="152">
+        <v>29</v>
+      </c>
+      <c r="C41" s="150" t="s">
+        <v>434</v>
+      </c>
+      <c r="D41" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E41" s="145"/>
+      <c r="F41" s="145" t="s">
+        <v>513</v>
+      </c>
+      <c r="G41" s="146"/>
+      <c r="H41" s="152">
+        <v>30</v>
+      </c>
+      <c r="I41" s="150" t="s">
+        <v>440</v>
+      </c>
+      <c r="J41" s="150" t="s">
+        <v>440</v>
+      </c>
+      <c r="K41" s="114"/>
+      <c r="L41" s="145" t="s">
+        <v>523</v>
+      </c>
+      <c r="M41" s="146"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B42" s="152">
+        <v>31</v>
+      </c>
+      <c r="C42" s="150" t="s">
+        <v>435</v>
+      </c>
+      <c r="D42" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E42" s="145"/>
+      <c r="F42" s="145" t="s">
+        <v>514</v>
+      </c>
+      <c r="G42" s="146"/>
+      <c r="H42" s="152">
+        <v>32</v>
+      </c>
+      <c r="I42" s="150" t="s">
+        <v>419</v>
+      </c>
+      <c r="J42" s="150" t="s">
+        <v>419</v>
+      </c>
+      <c r="K42" s="114"/>
+      <c r="L42" s="145" t="s">
+        <v>524</v>
+      </c>
+      <c r="M42" s="146"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B43" s="152">
+        <v>33</v>
+      </c>
+      <c r="C43" s="150" t="s">
+        <v>407</v>
+      </c>
+      <c r="D43" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E43" s="145"/>
+      <c r="F43" s="145" t="s">
+        <v>515</v>
+      </c>
+      <c r="G43" s="146"/>
+      <c r="H43" s="152">
+        <v>34</v>
+      </c>
+      <c r="I43" s="150" t="s">
+        <v>414</v>
+      </c>
+      <c r="J43" s="150" t="s">
+        <v>414</v>
+      </c>
+      <c r="K43" s="150" t="s">
+        <v>452</v>
+      </c>
+      <c r="L43" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M43" s="146"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B44" s="152">
+        <v>35</v>
+      </c>
+      <c r="C44" s="150" t="s">
+        <v>413</v>
+      </c>
+      <c r="D44" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E44" s="145"/>
+      <c r="F44" s="145" t="s">
+        <v>516</v>
+      </c>
+      <c r="G44" s="146"/>
+      <c r="H44" s="152">
+        <v>36</v>
+      </c>
+      <c r="I44" s="150" t="s">
+        <v>420</v>
+      </c>
+      <c r="J44" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K44" s="114"/>
+      <c r="L44" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M44" s="146"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B45" s="152">
+        <v>37</v>
+      </c>
+      <c r="C45" s="150" t="s">
+        <v>436</v>
+      </c>
+      <c r="D45" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="E45" s="145"/>
+      <c r="F45" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="G45" s="146"/>
+      <c r="H45" s="152">
+        <v>38</v>
+      </c>
+      <c r="I45" s="150" t="s">
         <v>423</v>
       </c>
-      <c r="D29" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E29" s="147"/>
-      <c r="F29" s="153">
-        <v>6</v>
-      </c>
-      <c r="G29" s="151" t="s">
-        <v>428</v>
-      </c>
-      <c r="H29" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I29" s="115"/>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="153">
-        <v>7</v>
-      </c>
-      <c r="C30" s="151" t="s">
-        <v>424</v>
-      </c>
-      <c r="D30" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E30" s="147"/>
-      <c r="F30" s="153">
-        <v>8</v>
-      </c>
-      <c r="G30" s="151" t="s">
-        <v>425</v>
-      </c>
-      <c r="H30" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I30" s="115"/>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B31" s="153">
-        <v>9</v>
-      </c>
-      <c r="C31" s="151" t="s">
-        <v>404</v>
-      </c>
-      <c r="D31" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E31" s="147"/>
-      <c r="F31" s="153">
-        <v>10</v>
-      </c>
-      <c r="G31" s="151" t="s">
-        <v>405</v>
-      </c>
-      <c r="H31" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I31" s="115"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B32" s="153">
-        <v>11</v>
-      </c>
-      <c r="C32" s="151" t="s">
-        <v>429</v>
-      </c>
-      <c r="D32" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E32" s="147"/>
-      <c r="F32" s="153">
-        <v>12</v>
-      </c>
-      <c r="G32" s="151" t="s">
-        <v>438</v>
-      </c>
-      <c r="H32" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I32" s="115"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="153">
-        <v>13</v>
-      </c>
-      <c r="C33" s="151" t="s">
-        <v>456</v>
-      </c>
-      <c r="D33" s="151" t="s">
-        <v>450</v>
-      </c>
-      <c r="E33" s="150" t="s">
-        <v>461</v>
-      </c>
-      <c r="F33" s="153">
-        <v>14</v>
-      </c>
-      <c r="G33" s="151" t="s">
-        <v>411</v>
-      </c>
-      <c r="H33" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I33" s="115"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="153">
-        <v>15</v>
-      </c>
-      <c r="C34" s="151" t="s">
-        <v>418</v>
-      </c>
-      <c r="D34" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E34" s="147"/>
-      <c r="F34" s="153">
-        <v>16</v>
-      </c>
-      <c r="G34" s="151" t="s">
-        <v>412</v>
-      </c>
-      <c r="H34" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I34" s="115"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="153">
-        <v>17</v>
-      </c>
-      <c r="C35" s="151" t="s">
-        <v>427</v>
-      </c>
-      <c r="D35" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E35" s="147"/>
-      <c r="F35" s="153">
-        <v>18</v>
-      </c>
-      <c r="G35" s="151" t="s">
-        <v>428</v>
-      </c>
-      <c r="H35" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I35" s="115"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="153">
-        <v>19</v>
-      </c>
-      <c r="C36" s="151" t="s">
-        <v>430</v>
-      </c>
-      <c r="D36" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E36" s="147"/>
-      <c r="F36" s="153">
-        <v>20</v>
-      </c>
-      <c r="G36" s="151" t="s">
-        <v>435</v>
-      </c>
-      <c r="H36" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I36" s="115"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="153">
-        <v>21</v>
-      </c>
-      <c r="C37" s="151" t="s">
-        <v>431</v>
-      </c>
-      <c r="D37" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E37" s="147"/>
-      <c r="F37" s="153">
-        <v>22</v>
-      </c>
-      <c r="G37" s="151" t="s">
-        <v>457</v>
-      </c>
-      <c r="H37" s="151" t="s">
-        <v>462</v>
-      </c>
-      <c r="I37" s="150" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="153">
-        <v>23</v>
-      </c>
-      <c r="C38" s="151" t="s">
-        <v>432</v>
-      </c>
-      <c r="D38" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E38" s="147"/>
-      <c r="F38" s="153">
-        <v>24</v>
-      </c>
-      <c r="G38" s="151" t="s">
-        <v>458</v>
-      </c>
-      <c r="H38" s="151" t="s">
-        <v>463</v>
-      </c>
-      <c r="I38" s="150" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="153">
-        <v>25</v>
-      </c>
-      <c r="C39" s="151" t="s">
-        <v>430</v>
-      </c>
-      <c r="D39" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E39" s="147"/>
-      <c r="F39" s="153">
-        <v>26</v>
-      </c>
-      <c r="G39" s="151" t="s">
-        <v>431</v>
-      </c>
-      <c r="H39" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I39" s="115"/>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="153">
-        <v>27</v>
-      </c>
-      <c r="C40" s="151" t="s">
-        <v>433</v>
-      </c>
-      <c r="D40" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E40" s="147"/>
-      <c r="F40" s="153">
-        <v>28</v>
-      </c>
-      <c r="G40" s="151" t="s">
-        <v>439</v>
-      </c>
-      <c r="H40" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I40" s="115"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="153">
-        <v>29</v>
-      </c>
-      <c r="C41" s="151" t="s">
-        <v>434</v>
-      </c>
-      <c r="D41" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E41" s="147"/>
-      <c r="F41" s="153">
-        <v>30</v>
-      </c>
-      <c r="G41" s="151" t="s">
-        <v>440</v>
-      </c>
-      <c r="H41" s="151" t="s">
-        <v>440</v>
-      </c>
-      <c r="I41" s="115"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="153">
-        <v>31</v>
-      </c>
-      <c r="C42" s="151" t="s">
-        <v>435</v>
-      </c>
-      <c r="D42" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E42" s="147"/>
-      <c r="F42" s="153">
-        <v>32</v>
-      </c>
-      <c r="G42" s="151" t="s">
-        <v>419</v>
-      </c>
-      <c r="H42" s="151" t="s">
-        <v>419</v>
-      </c>
-      <c r="I42" s="115"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="153">
-        <v>33</v>
-      </c>
-      <c r="C43" s="151" t="s">
-        <v>407</v>
-      </c>
-      <c r="D43" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E43" s="147"/>
-      <c r="F43" s="153">
-        <v>34</v>
-      </c>
-      <c r="G43" s="151" t="s">
-        <v>414</v>
-      </c>
-      <c r="H43" s="151" t="s">
-        <v>414</v>
-      </c>
-      <c r="I43" s="150" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="153">
-        <v>35</v>
-      </c>
-      <c r="C44" s="151" t="s">
-        <v>413</v>
-      </c>
-      <c r="D44" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E44" s="147"/>
-      <c r="F44" s="153">
-        <v>36</v>
-      </c>
-      <c r="G44" s="151" t="s">
-        <v>420</v>
-      </c>
-      <c r="H44" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I44" s="115"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="153">
-        <v>37</v>
-      </c>
-      <c r="C45" s="151" t="s">
-        <v>436</v>
-      </c>
-      <c r="D45" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="E45" s="147"/>
-      <c r="F45" s="153">
-        <v>38</v>
-      </c>
-      <c r="G45" s="151" t="s">
-        <v>423</v>
-      </c>
-      <c r="H45" s="146" t="s">
-        <v>444</v>
-      </c>
-      <c r="I45" s="115"/>
-    </row>
-    <row r="46" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="154">
+      <c r="J45" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="K45" s="114"/>
+      <c r="L45" s="145" t="s">
+        <v>443</v>
+      </c>
+      <c r="M45" s="146"/>
+    </row>
+    <row r="46" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="153">
         <v>39</v>
       </c>
-      <c r="C46" s="152" t="s">
+      <c r="C46" s="151" t="s">
         <v>437</v>
       </c>
-      <c r="D46" s="148" t="s">
-        <v>444</v>
-      </c>
-      <c r="E46" s="149"/>
-      <c r="F46" s="154">
+      <c r="D46" s="147" t="s">
+        <v>443</v>
+      </c>
+      <c r="E46" s="147"/>
+      <c r="F46" s="147" t="s">
+        <v>443</v>
+      </c>
+      <c r="G46" s="148"/>
+      <c r="H46" s="153">
         <v>40</v>
       </c>
-      <c r="G46" s="152" t="s">
+      <c r="I46" s="151" t="s">
         <v>441</v>
       </c>
-      <c r="H46" s="148" t="s">
-        <v>444</v>
-      </c>
-      <c r="I46" s="117"/>
+      <c r="J46" s="147" t="s">
+        <v>443</v>
+      </c>
+      <c r="K46" s="116"/>
+      <c r="L46" s="147" t="s">
+        <v>443</v>
+      </c>
+      <c r="M46" s="148"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>